<commit_message>
Read and write excel sheet
</commit_message>
<xml_diff>
--- a/Resource/Book1.xlsx
+++ b/Resource/Book1.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView windowHeight="7995" windowWidth="20115" xWindow="240" yWindow="75"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
+    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -24,16 +24,35 @@
     <t>password</t>
   </si>
   <si>
-    <t>Saurab@gmail.com</t>
-  </si>
-  <si>
     <t>test@123</t>
+  </si>
+  <si>
+    <t>Amol@gmail.com</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Chandu@gmail.com</t>
+  </si>
+  <si>
+    <t>pass1123</t>
+  </si>
+  <si>
+    <t>Azhar@gmail.com</t>
+  </si>
+  <si>
+    <t>test345</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -77,20 +96,20 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -104,10 +123,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -265,7 +284,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -274,13 +293,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -290,7 +309,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -299,7 +318,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -308,7 +327,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -318,12 +337,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -354,7 +373,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -373,7 +392,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -385,64 +404,89 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="16.85546875" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="14.0" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink r:id="rId2" ref="A2"/>
+    <hyperlink r:id="rId3" ref="A3"/>
+    <hyperlink r:id="rId4" ref="A4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="200" orientation="portrait" r:id="rId5" verticalDpi="200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>